<commit_message>
updated xl file for asset upload
</commit_message>
<xml_diff>
--- a/Audit_Code/public/assets_template.xlsx
+++ b/Audit_Code/public/assets_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ab\Desktop\Compliance\Audit_Code\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,9 +29,6 @@
     <t>Asset Group Name</t>
   </si>
   <si>
-    <t>Asset Name</t>
-  </si>
-  <si>
     <t>Asset Component Name</t>
   </si>
   <si>
@@ -44,7 +41,10 @@
     <t>Asset Logical Location</t>
   </si>
   <si>
-    <t>Service Name for which this is an underlying asset</t>
+    <t>Service Name</t>
+  </si>
+  <si>
+    <t>Asset  Name</t>
   </si>
 </sst>
 </file>
@@ -364,9 +364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -381,25 +379,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>